<commit_message>
complete nrc report assistant win
</commit_message>
<xml_diff>
--- a/MH_NRC_Report_2023_08_05_11_10_39.xlsx
+++ b/MH_NRC_Report_2023_08_05_11_10_39.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
-  <si>
-    <t>Nrc_Id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
+  <si>
+    <t>NRC_ID</t>
   </si>
   <si>
     <t>Register</t>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>ZONE C SEAT 56B 57C 59A 59B 61A 61B 65C 66B 67B 66D 64D 64F 63D 62F 62D 61F 59F 57E 57G 56E 54G 55K 56J 59H 59J 61J 61H 62H64H 64K MONITOR TOUCHSCREEN FOUND MALFUNCTION</t>
+  </si>
+  <si>
+    <t>QZL0070</t>
   </si>
 </sst>
 </file>
@@ -158,7 +161,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,13 +172,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -643,48 +639,51 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -694,97 +693,94 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1139,14 +1135,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7"/>
   <cols>
+    <col min="3" max="3" width="25.4444444444444" customWidth="1"/>
     <col min="10" max="10" width="7.22222222222222" customWidth="1"/>
     <col min="11" max="11" width="13.1111111111111" customWidth="1"/>
   </cols>
@@ -1396,6 +1393,41 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8">
+        <v>50</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>